<commit_message>
Work on team 1-3.
</commit_message>
<xml_diff>
--- a/models/mini_fixedwing_02/team02.xlsx
+++ b/models/mini_fixedwing_02/team02.xlsx
@@ -581,7 +581,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -604,6 +604,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF2F929A"/>
         <bgColor rgb="FF008080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF72BF44"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
     <fill>
@@ -653,7 +659,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -734,6 +740,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -742,11 +756,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -815,7 +833,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF4285F4"/>
       <rgbColor rgb="FF46BDC6"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF72BF44"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -841,13 +859,13 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>123840</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>228240</xdr:colOff>
+      <xdr:colOff>227880</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>58680</xdr:rowOff>
+      <xdr:rowOff>114120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -860,8 +878,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11172600" y="6238800"/>
-          <a:ext cx="6114600" cy="3790440"/>
+          <a:off x="11166840" y="6238800"/>
+          <a:ext cx="6110640" cy="3790080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -878,13 +896,13 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>29160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>342720</xdr:colOff>
+      <xdr:colOff>342360</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>12960</xdr:rowOff>
+      <xdr:rowOff>53280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -897,8 +915,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11172600" y="3786840"/>
-          <a:ext cx="6229080" cy="2676240"/>
+          <a:off x="11166840" y="3786840"/>
+          <a:ext cx="6225120" cy="2675880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -920,16 +938,16 @@
   </sheetPr>
   <dimension ref="A1:Z228"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C213" activeCellId="0" sqref="C213"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A148" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D178" activeCellId="0" sqref="D178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1341,7 +1359,7 @@
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="14" t="n">
+      <c r="B13" s="20" t="n">
         <v>-0.051</v>
       </c>
       <c r="C13" s="14" t="n">
@@ -1387,7 +1405,7 @@
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="14" t="n">
+      <c r="B14" s="20" t="n">
         <v>0.211</v>
       </c>
       <c r="C14" s="6"/>
@@ -1467,33 +1485,33 @@
       <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="20" t="n">
+      <c r="B16" s="21" t="n">
         <f aca="false">2022106.96*10^-9</f>
         <v>0.00202210696</v>
       </c>
-      <c r="C16" s="20" t="n">
+      <c r="C16" s="22" t="n">
         <f aca="false">208745.9*10^-9</f>
         <v>0.0002087459</v>
       </c>
-      <c r="D16" s="20" t="n">
+      <c r="D16" s="22" t="n">
         <f aca="false">1504*10^-9</f>
         <v>1.504E-006</v>
       </c>
-      <c r="E16" s="20" t="n">
+      <c r="E16" s="21" t="n">
         <f aca="false">4989227.9*10^-9</f>
         <v>0.0049892279</v>
       </c>
-      <c r="F16" s="20" t="n">
+      <c r="F16" s="22" t="n">
         <f aca="false">-609*10^-9</f>
         <v>-6.09E-007</v>
       </c>
-      <c r="G16" s="20" t="n">
+      <c r="G16" s="21" t="n">
         <f aca="false">3099700*10^-9</f>
         <v>0.0030997</v>
       </c>
       <c r="H16" s="6"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
@@ -1575,7 +1593,7 @@
       <c r="Y18" s="6"/>
       <c r="Z18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
@@ -1608,7 +1626,7 @@
       <c r="Y19" s="6"/>
       <c r="Z19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1636,7 +1654,7 @@
       <c r="Y20" s="6"/>
       <c r="Z20" s="6"/>
     </row>
-    <row r="21" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
         <v>45</v>
       </c>
@@ -1644,7 +1662,7 @@
       <c r="C21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="24" t="s">
         <v>47</v>
       </c>
       <c r="F21" s="6"/>
@@ -1671,7 +1689,7 @@
       <c r="Y21" s="6"/>
       <c r="Z21" s="6"/>
     </row>
-    <row r="22" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7"/>
       <c r="B22" s="2" t="s">
         <v>10</v>
@@ -1711,17 +1729,17 @@
       <c r="Y22" s="6"/>
       <c r="Z22" s="6"/>
     </row>
-    <row r="23" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="14" t="n">
+      <c r="B23" s="20" t="n">
         <v>-0.072</v>
       </c>
-      <c r="C23" s="23" t="n">
+      <c r="C23" s="25" t="n">
         <v>-0.066</v>
       </c>
-      <c r="D23" s="14" t="n">
+      <c r="D23" s="20" t="n">
         <v>-0.039</v>
       </c>
       <c r="E23" s="14" t="n">
@@ -1749,7 +1767,7 @@
       <c r="Y23" s="6"/>
       <c r="Z23" s="6"/>
     </row>
-    <row r="24" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
         <v>19</v>
       </c>
@@ -1787,7 +1805,7 @@
       <c r="Y24" s="6"/>
       <c r="Z24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
@@ -1829,7 +1847,7 @@
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="14" t="n">
+      <c r="B26" s="20" t="n">
         <v>0.001</v>
       </c>
       <c r="C26" s="2"/>
@@ -1889,11 +1907,11 @@
       <c r="Y27" s="6"/>
       <c r="Z27" s="6"/>
     </row>
-    <row r="28" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="20" t="n">
+      <c r="B28" s="26" t="n">
         <v>1E-006</v>
       </c>
       <c r="C28" s="14" t="n">
@@ -1902,13 +1920,13 @@
       <c r="D28" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="E28" s="20" t="n">
+      <c r="E28" s="26" t="n">
         <v>1E-007</v>
       </c>
       <c r="F28" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="G28" s="20" t="n">
+      <c r="G28" s="26" t="n">
         <v>1E-006</v>
       </c>
       <c r="H28" s="6"/>
@@ -2027,7 +2045,7 @@
       <c r="A32" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="14" t="n">
+      <c r="B32" s="25" t="n">
         <v>0.032</v>
       </c>
       <c r="C32" s="2"/>
@@ -2059,7 +2077,7 @@
       <c r="A33" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="14" t="n">
+      <c r="B33" s="20" t="n">
         <v>0.01</v>
       </c>
       <c r="C33" s="2"/>
@@ -2123,7 +2141,7 @@
       <c r="C35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="D35" s="24" t="s">
         <v>47</v>
       </c>
       <c r="F35" s="6"/>
@@ -2194,13 +2212,13 @@
       <c r="A37" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="14" t="n">
+      <c r="B37" s="20" t="n">
         <v>-0.07</v>
       </c>
-      <c r="C37" s="23" t="n">
+      <c r="C37" s="25" t="n">
         <v>0.066</v>
       </c>
-      <c r="D37" s="14" t="n">
+      <c r="D37" s="20" t="n">
         <v>-0.039</v>
       </c>
       <c r="E37" s="14" t="n">
@@ -2320,7 +2338,7 @@
       <c r="A40" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="14" t="n">
+      <c r="B40" s="20" t="n">
         <v>0.001</v>
       </c>
       <c r="C40" s="2"/>
@@ -2388,11 +2406,11 @@
       <c r="Y41" s="6"/>
       <c r="Z41" s="6"/>
     </row>
-    <row r="42" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="20" t="n">
+      <c r="B42" s="26" t="n">
         <v>1E-006</v>
       </c>
       <c r="C42" s="14" t="n">
@@ -2401,13 +2419,13 @@
       <c r="D42" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="E42" s="20" t="n">
+      <c r="E42" s="26" t="n">
         <v>1E-007</v>
       </c>
       <c r="F42" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="G42" s="20" t="n">
+      <c r="G42" s="26" t="n">
         <v>1E-006</v>
       </c>
       <c r="H42" s="6"/>
@@ -2462,7 +2480,7 @@
       <c r="Y43" s="6"/>
       <c r="Z43" s="6"/>
     </row>
-    <row r="44" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
         <v>40</v>
       </c>
@@ -2530,7 +2548,7 @@
       <c r="A46" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="14" t="n">
+      <c r="B46" s="25" t="n">
         <v>0.032</v>
       </c>
       <c r="C46" s="2"/>
@@ -2562,7 +2580,7 @@
       <c r="A47" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="14" t="n">
+      <c r="B47" s="20" t="n">
         <v>0.01</v>
       </c>
       <c r="C47" s="2"/>
@@ -2618,7 +2636,7 @@
       <c r="Y48" s="6"/>
       <c r="Z48" s="6"/>
     </row>
-    <row r="49" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="7" t="s">
         <v>56</v>
       </c>
@@ -2626,7 +2644,7 @@
       <c r="C49" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D49" s="22" t="s">
+      <c r="D49" s="24" t="s">
         <v>57</v>
       </c>
       <c r="F49" s="6"/>
@@ -2799,7 +2817,7 @@
       <c r="A54" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B54" s="14" t="n">
+      <c r="B54" s="20" t="n">
         <v>0.001</v>
       </c>
       <c r="C54" s="2"/>
@@ -2859,7 +2877,7 @@
       <c r="A56" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B56" s="20" t="n">
+      <c r="B56" s="22" t="n">
         <v>1E-006</v>
       </c>
       <c r="C56" s="14" t="n">
@@ -2868,16 +2886,16 @@
       <c r="D56" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="E56" s="20" t="n">
+      <c r="E56" s="22" t="n">
         <v>1E-007</v>
       </c>
       <c r="F56" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="G56" s="20" t="n">
+      <c r="G56" s="22" t="n">
         <v>1E-006</v>
       </c>
-      <c r="K56" s="24" t="s">
+      <c r="K56" s="27" t="s">
         <v>58</v>
       </c>
       <c r="N56" s="6"/>
@@ -2906,7 +2924,7 @@
       <c r="E57" s="7"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
-      <c r="K57" s="24" t="s">
+      <c r="K57" s="27" t="s">
         <v>60</v>
       </c>
       <c r="N57" s="6"/>
@@ -2935,7 +2953,7 @@
       <c r="E58" s="7"/>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
-      <c r="K58" s="25"/>
+      <c r="K58" s="28"/>
       <c r="N58" s="6"/>
       <c r="O58" s="6"/>
       <c r="P58" s="6"/>
@@ -2980,7 +2998,7 @@
       <c r="A60" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B60" s="14" t="n">
+      <c r="B60" s="20" t="n">
         <v>0.025</v>
       </c>
       <c r="C60" s="2"/>
@@ -3006,7 +3024,7 @@
       <c r="A61" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="14" t="n">
+      <c r="B61" s="20" t="n">
         <v>0.02</v>
       </c>
       <c r="C61" s="2"/>
@@ -3051,7 +3069,7 @@
       <c r="C63" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D63" s="22" t="s">
+      <c r="D63" s="24" t="s">
         <v>47</v>
       </c>
       <c r="F63" s="6"/>
@@ -3113,13 +3131,13 @@
       <c r="A65" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B65" s="14" t="n">
+      <c r="B65" s="20" t="n">
         <v>-0.406</v>
       </c>
       <c r="C65" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="D65" s="14" t="n">
+      <c r="D65" s="20" t="n">
         <v>0.038</v>
       </c>
       <c r="E65" s="14" t="n">
@@ -3187,7 +3205,7 @@
       <c r="A67" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B67" s="14" t="n">
+      <c r="B67" s="20" t="n">
         <v>-0.02</v>
       </c>
       <c r="C67" s="14" t="n">
@@ -3296,7 +3314,7 @@
       <c r="A70" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B70" s="20" t="n">
+      <c r="B70" s="21" t="n">
         <v>1E-006</v>
       </c>
       <c r="C70" s="14" t="n">
@@ -3305,13 +3323,13 @@
       <c r="D70" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="E70" s="20" t="n">
+      <c r="E70" s="21" t="n">
         <v>1E-006</v>
       </c>
       <c r="F70" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="G70" s="20" t="n">
+      <c r="G70" s="21" t="n">
         <v>1E-006</v>
       </c>
       <c r="H70" s="6"/>
@@ -3522,7 +3540,7 @@
       <c r="C77" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D77" s="22" t="s">
+      <c r="D77" s="24" t="s">
         <v>47</v>
       </c>
       <c r="F77" s="6"/>
@@ -3591,13 +3609,13 @@
       <c r="A79" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B79" s="14" t="n">
+      <c r="B79" s="20" t="n">
         <v>-0.431</v>
       </c>
       <c r="C79" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="D79" s="14" t="n">
+      <c r="D79" s="20" t="n">
         <v>0.038</v>
       </c>
       <c r="E79" s="14" t="n">
@@ -3673,7 +3691,7 @@
       <c r="A81" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B81" s="14" t="n">
+      <c r="B81" s="20" t="n">
         <v>-0.02</v>
       </c>
       <c r="C81" s="14" t="n">
@@ -3712,7 +3730,7 @@
       <c r="A82" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B82" s="14" t="n">
+      <c r="B82" s="20" t="n">
         <v>0.001</v>
       </c>
       <c r="C82" s="2"/>
@@ -3777,7 +3795,7 @@
       <c r="A84" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B84" s="20" t="n">
+      <c r="B84" s="21" t="n">
         <v>1E-006</v>
       </c>
       <c r="C84" s="14" t="n">
@@ -3786,13 +3804,13 @@
       <c r="D84" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="E84" s="20" t="n">
+      <c r="E84" s="21" t="n">
         <v>1E-006</v>
       </c>
       <c r="F84" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="G84" s="20" t="n">
+      <c r="G84" s="21" t="n">
         <v>1E-006</v>
       </c>
       <c r="L84" s="6"/>
@@ -3867,7 +3885,7 @@
       <c r="Y86" s="6"/>
       <c r="Z86" s="6"/>
     </row>
-    <row r="87" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
         <v>63</v>
       </c>
@@ -3876,7 +3894,9 @@
       </c>
       <c r="C87" s="6"/>
       <c r="D87" s="6"/>
-      <c r="E87" s="6"/>
+      <c r="E87" s="6" t="n">
+        <v>0.026</v>
+      </c>
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
       <c r="L87" s="6"/>
@@ -3924,7 +3944,7 @@
       <c r="Z88" s="6"/>
     </row>
     <row r="89" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="24" t="s">
+      <c r="A89" s="27" t="s">
         <v>42</v>
       </c>
       <c r="B89" s="14" t="s">
@@ -3971,7 +3991,7 @@
       <c r="C91" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D91" s="22" t="s">
+      <c r="D91" s="24" t="s">
         <v>47</v>
       </c>
       <c r="F91" s="6"/>
@@ -4035,13 +4055,13 @@
       <c r="A93" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B93" s="14" t="n">
+      <c r="B93" s="20" t="n">
         <v>-0.196</v>
       </c>
-      <c r="C93" s="14" t="n">
+      <c r="C93" s="20" t="n">
         <v>0.235</v>
       </c>
-      <c r="D93" s="14" t="n">
+      <c r="D93" s="20" t="n">
         <v>0.035</v>
       </c>
       <c r="E93" s="14" t="n">
@@ -4111,7 +4131,7 @@
       <c r="A95" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B95" s="14" t="n">
+      <c r="B95" s="20" t="n">
         <v>-0.02</v>
       </c>
       <c r="C95" s="14" t="n">
@@ -4149,7 +4169,7 @@
       <c r="A96" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B96" s="14" t="n">
+      <c r="B96" s="20" t="n">
         <v>0.001</v>
       </c>
       <c r="C96" s="2"/>
@@ -4213,7 +4233,7 @@
       <c r="A98" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B98" s="20" t="n">
+      <c r="B98" s="21" t="n">
         <v>1E-006</v>
       </c>
       <c r="C98" s="14" t="n">
@@ -4222,13 +4242,13 @@
       <c r="D98" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="E98" s="20" t="n">
+      <c r="E98" s="21" t="n">
         <v>1E-006</v>
       </c>
       <c r="F98" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="G98" s="20" t="n">
+      <c r="G98" s="21" t="n">
         <v>1E-006</v>
       </c>
       <c r="L98" s="6"/>
@@ -4360,7 +4380,7 @@
       <c r="Z102" s="6"/>
     </row>
     <row r="103" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="24" t="s">
+      <c r="A103" s="27" t="s">
         <v>42</v>
       </c>
       <c r="B103" s="14" t="s">
@@ -4407,7 +4427,7 @@
       <c r="C105" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D105" s="22" t="s">
+      <c r="D105" s="24" t="s">
         <v>47</v>
       </c>
       <c r="F105" s="6"/>
@@ -4471,13 +4491,13 @@
       <c r="A107" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B107" s="14" t="n">
+      <c r="B107" s="20" t="n">
         <v>-0.196</v>
       </c>
-      <c r="C107" s="14" t="n">
+      <c r="C107" s="20" t="n">
         <v>-0.235</v>
       </c>
-      <c r="D107" s="14" t="n">
+      <c r="D107" s="20" t="n">
         <v>0.035</v>
       </c>
       <c r="E107" s="14" t="n">
@@ -4543,7 +4563,7 @@
       <c r="A109" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B109" s="14" t="n">
+      <c r="B109" s="20" t="n">
         <v>-0.02</v>
       </c>
       <c r="C109" s="14" t="n">
@@ -4579,7 +4599,7 @@
       <c r="A110" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B110" s="14" t="n">
+      <c r="B110" s="20" t="n">
         <v>0.001</v>
       </c>
       <c r="C110" s="2"/>
@@ -4639,7 +4659,7 @@
       <c r="A112" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B112" s="20" t="n">
+      <c r="B112" s="21" t="n">
         <v>1E-006</v>
       </c>
       <c r="C112" s="14" t="n">
@@ -4648,13 +4668,13 @@
       <c r="D112" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="E112" s="20" t="n">
+      <c r="E112" s="21" t="n">
         <v>1E-006</v>
       </c>
       <c r="F112" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="G112" s="20" t="n">
+      <c r="G112" s="21" t="n">
         <v>1E-006</v>
       </c>
       <c r="N112" s="6"/>
@@ -4776,7 +4796,7 @@
       <c r="Z116" s="6"/>
     </row>
     <row r="117" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="24" t="s">
+      <c r="A117" s="27" t="s">
         <v>42</v>
       </c>
       <c r="B117" s="14" t="s">
@@ -4841,7 +4861,7 @@
       <c r="A120" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B120" s="14" t="n">
+      <c r="B120" s="20" t="n">
         <v>0</v>
       </c>
       <c r="C120" s="6"/>
@@ -4873,7 +4893,7 @@
       <c r="A121" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B121" s="14" t="n">
+      <c r="B121" s="20" t="n">
         <v>6.28</v>
       </c>
       <c r="C121" s="6"/>
@@ -4901,7 +4921,7 @@
       <c r="Y121" s="6"/>
       <c r="Z121" s="6"/>
     </row>
-    <row r="122" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2" t="s">
         <v>79</v>
       </c>
@@ -4937,7 +4957,7 @@
       <c r="A123" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B123" s="14" t="n">
+      <c r="B123" s="20" t="n">
         <v>-0.315</v>
       </c>
       <c r="C123" s="6"/>
@@ -4969,7 +4989,7 @@
       <c r="A124" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B124" s="14" t="n">
+      <c r="B124" s="20" t="n">
         <v>0.175</v>
       </c>
       <c r="C124" s="6"/>
@@ -5001,7 +5021,7 @@
       <c r="A125" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B125" s="14" t="n">
+      <c r="B125" s="20" t="n">
         <v>-6.2</v>
       </c>
       <c r="C125" s="6"/>
@@ -5065,7 +5085,7 @@
       <c r="A127" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B127" s="14" t="n">
+      <c r="B127" s="20" t="n">
         <v>0</v>
       </c>
       <c r="C127" s="6"/>
@@ -5093,11 +5113,11 @@
       <c r="Y127" s="6"/>
       <c r="Z127" s="6"/>
     </row>
-    <row r="128" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B128" s="14" t="n">
+      <c r="B128" s="25" t="n">
         <v>-0.305</v>
       </c>
       <c r="C128" s="14" t="n">
@@ -5133,7 +5153,7 @@
       <c r="A129" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B129" s="14" t="n">
+      <c r="B129" s="20" t="n">
         <v>0.006</v>
       </c>
       <c r="C129" s="6"/>
@@ -5165,13 +5185,13 @@
       <c r="A130" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B130" s="14" t="n">
+      <c r="B130" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="C130" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D130" s="14" t="n">
+      <c r="C130" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D130" s="20" t="n">
         <v>0</v>
       </c>
       <c r="E130" s="6"/>
@@ -5201,13 +5221,13 @@
       <c r="A131" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B131" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C131" s="14" t="n">
+      <c r="B131" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C131" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D131" s="14" t="n">
+      <c r="D131" s="20" t="n">
         <v>0</v>
       </c>
       <c r="E131" s="6"/>
@@ -5237,7 +5257,7 @@
       <c r="A132" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B132" s="14" t="n">
+      <c r="B132" s="20" t="n">
         <v>4</v>
       </c>
       <c r="C132" s="6"/>
@@ -5318,7 +5338,7 @@
       <c r="A135" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B135" s="14" t="n">
+      <c r="B135" s="20" t="n">
         <v>0</v>
       </c>
       <c r="C135" s="6"/>
@@ -5348,7 +5368,7 @@
       <c r="A136" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B136" s="14" t="n">
+      <c r="B136" s="20" t="n">
         <v>6.51</v>
       </c>
       <c r="C136" s="6"/>
@@ -5408,7 +5428,7 @@
       <c r="A138" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B138" s="14" t="n">
+      <c r="B138" s="20" t="n">
         <v>-0.381</v>
       </c>
       <c r="C138" s="6"/>
@@ -5438,7 +5458,7 @@
       <c r="A139" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B139" s="14" t="n">
+      <c r="B139" s="20" t="n">
         <v>0.198</v>
       </c>
       <c r="C139" s="6"/>
@@ -5466,7 +5486,7 @@
       <c r="A140" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B140" s="14" t="n">
+      <c r="B140" s="20" t="n">
         <v>-6.51</v>
       </c>
       <c r="C140" s="6"/>
@@ -5556,7 +5576,7 @@
       <c r="A143" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B143" s="14" t="n">
+      <c r="B143" s="25" t="n">
         <v>-0.3</v>
       </c>
       <c r="C143" s="14" t="n">
@@ -5590,7 +5610,7 @@
       <c r="A144" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B144" s="14" t="n">
+      <c r="B144" s="20" t="n">
         <v>0.0217</v>
       </c>
       <c r="C144" s="6"/>
@@ -5620,13 +5640,13 @@
       <c r="A145" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B145" s="14" t="n">
+      <c r="B145" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="C145" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D145" s="14" t="n">
+      <c r="C145" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D145" s="20" t="n">
         <v>0</v>
       </c>
       <c r="E145" s="6"/>
@@ -5654,13 +5674,13 @@
       <c r="A146" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B146" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C146" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D146" s="14" t="n">
+      <c r="B146" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C146" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D146" s="20" t="n">
         <v>1</v>
       </c>
       <c r="E146" s="6"/>
@@ -5688,7 +5708,7 @@
       <c r="A147" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B147" s="14" t="n">
+      <c r="B147" s="20" t="n">
         <v>-4</v>
       </c>
       <c r="C147" s="6"/>
@@ -5759,7 +5779,7 @@
       <c r="A150" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B150" s="14" t="n">
+      <c r="B150" s="20" t="n">
         <v>0</v>
       </c>
       <c r="C150" s="6"/>
@@ -5790,7 +5810,7 @@
       <c r="A151" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B151" s="14" t="n">
+      <c r="B151" s="20" t="n">
         <v>6.322</v>
       </c>
       <c r="C151" s="6"/>
@@ -5852,7 +5872,7 @@
       <c r="A153" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B153" s="14" t="n">
+      <c r="B153" s="20" t="n">
         <v>-0.381</v>
       </c>
       <c r="C153" s="6"/>
@@ -5883,7 +5903,7 @@
       <c r="A154" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B154" s="14" t="n">
+      <c r="B154" s="20" t="n">
         <v>0.275</v>
       </c>
       <c r="C154" s="6"/>
@@ -5913,7 +5933,7 @@
       <c r="A155" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B155" s="14" t="n">
+      <c r="B155" s="20" t="n">
         <v>-6.3</v>
       </c>
       <c r="C155" s="6"/>
@@ -5973,7 +5993,7 @@
       <c r="A157" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B157" s="14" t="n">
+      <c r="B157" s="20" t="n">
         <v>0</v>
       </c>
       <c r="C157" s="6"/>
@@ -6003,13 +6023,13 @@
       <c r="A158" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B158" s="14" t="n">
+      <c r="B158" s="20" t="n">
         <v>-0.11</v>
       </c>
-      <c r="C158" s="14" t="n">
+      <c r="C158" s="20" t="n">
         <v>0.178</v>
       </c>
-      <c r="D158" s="14" t="n">
+      <c r="D158" s="20" t="n">
         <v>0</v>
       </c>
       <c r="E158" s="6"/>
@@ -6037,7 +6057,7 @@
       <c r="A159" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B159" s="14" t="n">
+      <c r="B159" s="20" t="n">
         <v>0.0387</v>
       </c>
       <c r="C159" s="6"/>
@@ -6067,13 +6087,13 @@
       <c r="A160" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B160" s="14" t="n">
+      <c r="B160" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="C160" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D160" s="14" t="n">
+      <c r="C160" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D160" s="20" t="n">
         <v>0</v>
       </c>
       <c r="E160" s="6"/>
@@ -6101,13 +6121,13 @@
       <c r="A161" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B161" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C161" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D161" s="14" t="n">
+      <c r="B161" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C161" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D161" s="20" t="n">
         <v>1</v>
       </c>
       <c r="E161" s="6"/>
@@ -6135,7 +6155,7 @@
       <c r="A162" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B162" s="14" t="n">
+      <c r="B162" s="20" t="n">
         <v>-2</v>
       </c>
       <c r="C162" s="6"/>
@@ -6208,7 +6228,7 @@
       <c r="A165" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B165" s="14" t="n">
+      <c r="B165" s="20" t="n">
         <v>0</v>
       </c>
       <c r="C165" s="6"/>
@@ -6239,7 +6259,7 @@
       <c r="A166" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B166" s="14" t="n">
+      <c r="B166" s="20" t="n">
         <v>6.322</v>
       </c>
       <c r="C166" s="6"/>
@@ -6301,7 +6321,7 @@
       <c r="A168" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B168" s="14" t="n">
+      <c r="B168" s="20" t="n">
         <v>-0.381</v>
       </c>
       <c r="C168" s="6"/>
@@ -6332,7 +6352,7 @@
       <c r="A169" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B169" s="14" t="n">
+      <c r="B169" s="20" t="n">
         <v>0.275</v>
       </c>
       <c r="C169" s="6"/>
@@ -6362,7 +6382,7 @@
       <c r="A170" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B170" s="14" t="n">
+      <c r="B170" s="20" t="n">
         <v>-6.3</v>
       </c>
       <c r="C170" s="6"/>
@@ -6422,7 +6442,7 @@
       <c r="A172" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B172" s="14" t="n">
+      <c r="B172" s="20" t="n">
         <v>0</v>
       </c>
       <c r="C172" s="6"/>
@@ -6452,13 +6472,13 @@
       <c r="A173" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B173" s="14" t="n">
+      <c r="B173" s="20" t="n">
         <v>-0.11</v>
       </c>
-      <c r="C173" s="14" t="n">
+      <c r="C173" s="20" t="n">
         <v>-0.178</v>
       </c>
-      <c r="D173" s="14" t="n">
+      <c r="D173" s="20" t="n">
         <v>0</v>
       </c>
       <c r="E173" s="6"/>
@@ -6486,7 +6506,7 @@
       <c r="A174" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B174" s="14" t="n">
+      <c r="B174" s="20" t="n">
         <v>0.0387</v>
       </c>
       <c r="C174" s="6"/>
@@ -6516,13 +6536,13 @@
       <c r="A175" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B175" s="14" t="n">
+      <c r="B175" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="C175" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D175" s="14" t="n">
+      <c r="C175" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D175" s="20" t="n">
         <v>0</v>
       </c>
       <c r="E175" s="6"/>
@@ -6550,13 +6570,13 @@
       <c r="A176" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B176" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C176" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D176" s="14" t="n">
+      <c r="B176" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C176" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D176" s="20" t="n">
         <v>1</v>
       </c>
       <c r="E176" s="6"/>
@@ -6584,7 +6604,7 @@
       <c r="A177" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B177" s="14" t="n">
+      <c r="B177" s="20" t="n">
         <v>-2</v>
       </c>
       <c r="C177" s="6"/>
@@ -6692,13 +6712,13 @@
       <c r="A181" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B181" s="14" t="n">
+      <c r="B181" s="20" t="n">
         <v>-0.028</v>
       </c>
       <c r="C181" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="D181" s="14" t="n">
+      <c r="D181" s="20" t="n">
         <v>0.017</v>
       </c>
       <c r="E181" s="14" t="n">
@@ -6809,7 +6829,7 @@
       <c r="A184" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B184" s="14" t="n">
+      <c r="B184" s="20" t="n">
         <v>0.0071</v>
       </c>
       <c r="C184" s="2"/>
@@ -6876,24 +6896,24 @@
       <c r="A186" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B186" s="20" t="n">
+      <c r="B186" s="21" t="n">
         <f aca="false">723*10^-9</f>
         <v>7.23E-007</v>
       </c>
-      <c r="C186" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="D186" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="E186" s="20" t="n">
+      <c r="C186" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D186" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E186" s="21" t="n">
         <f aca="false">7725*10^-9</f>
         <v>7.725E-006</v>
       </c>
-      <c r="F186" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="G186" s="20" t="n">
+      <c r="F186" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G186" s="21" t="n">
         <f aca="false">8300*10^-9</f>
         <v>8.3E-006</v>
       </c>
@@ -6976,7 +6996,7 @@
       <c r="Z188" s="6"/>
     </row>
     <row r="189" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="24" t="s">
+      <c r="A189" s="27" t="s">
         <v>42</v>
       </c>
       <c r="B189" s="14" t="s">
@@ -7001,7 +7021,7 @@
       <c r="Z189" s="6"/>
     </row>
     <row r="190" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="24" t="s">
+      <c r="A190" s="27" t="s">
         <v>109</v>
       </c>
       <c r="B190" s="14" t="n">
@@ -7026,7 +7046,7 @@
       <c r="Z190" s="6"/>
     </row>
     <row r="191" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="26" t="s">
+      <c r="A191" s="29" t="s">
         <v>110</v>
       </c>
       <c r="B191" s="14" t="n">
@@ -7054,28 +7074,28 @@
       <c r="Z191" s="6"/>
     </row>
     <row r="192" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="26" t="s">
+      <c r="A192" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="B192" s="14" t="n">
+      <c r="B192" s="20" t="n">
         <v>0.1</v>
       </c>
-      <c r="C192" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D192" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E192" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F192" s="14" t="n">
+      <c r="C192" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D192" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E192" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F192" s="20" t="n">
         <v>0</v>
       </c>
       <c r="I192" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="J192" s="21"/>
+      <c r="J192" s="23"/>
       <c r="K192" s="6"/>
       <c r="L192" s="6"/>
       <c r="M192" s="6"/>
@@ -7094,28 +7114,28 @@
       <c r="Z192" s="6"/>
     </row>
     <row r="193" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="26" t="s">
+      <c r="A193" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="B193" s="14" t="n">
+      <c r="B193" s="20" t="n">
         <v>0.05</v>
       </c>
-      <c r="C193" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D193" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E193" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F193" s="14" t="n">
+      <c r="C193" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D193" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E193" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F193" s="20" t="n">
         <v>0</v>
       </c>
       <c r="I193" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="J193" s="21"/>
+      <c r="J193" s="23"/>
       <c r="K193" s="6"/>
       <c r="L193" s="6"/>
       <c r="M193" s="6"/>
@@ -7165,7 +7185,7 @@
       <c r="C195" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D195" s="22" t="s">
+      <c r="D195" s="24" t="s">
         <v>57</v>
       </c>
       <c r="F195" s="6"/>
@@ -7515,7 +7535,7 @@
       <c r="Z204" s="6"/>
     </row>
     <row r="205" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="24" t="s">
+      <c r="A205" s="27" t="s">
         <v>42</v>
       </c>
       <c r="B205" s="14" t="s">
@@ -7540,7 +7560,7 @@
       <c r="Z205" s="6"/>
     </row>
     <row r="206" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="24" t="s">
+      <c r="A206" s="27" t="s">
         <v>109</v>
       </c>
       <c r="B206" s="14" t="n">
@@ -7565,7 +7585,7 @@
       <c r="Z206" s="6"/>
     </row>
     <row r="207" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="26" t="s">
+      <c r="A207" s="29" t="s">
         <v>110</v>
       </c>
       <c r="B207" s="14" t="n">
@@ -7590,22 +7610,22 @@
       <c r="Z207" s="6"/>
     </row>
     <row r="208" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="26" t="s">
+      <c r="A208" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="B208" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="C208" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="D208" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="E208" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="F208" s="23" t="n">
+      <c r="B208" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C208" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D208" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E208" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F208" s="14" t="n">
         <v>0</v>
       </c>
       <c r="I208" s="18"/>
@@ -7628,22 +7648,22 @@
       <c r="Z208" s="6"/>
     </row>
     <row r="209" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="26" t="s">
+      <c r="A209" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="B209" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="C209" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="D209" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="E209" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="F209" s="23" t="n">
+      <c r="B209" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C209" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D209" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E209" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F209" s="14" t="n">
         <v>0</v>
       </c>
       <c r="I209" s="18"/>
@@ -8107,10 +8127,10 @@
       <c r="Z223" s="6"/>
     </row>
     <row r="224" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="26" t="s">
+      <c r="A224" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="B224" s="14" t="n">
+      <c r="B224" s="20" t="n">
         <v>2200</v>
       </c>
       <c r="I224" s="18" t="s">
@@ -8131,10 +8151,10 @@
       <c r="Z224" s="6"/>
     </row>
     <row r="225" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="26" t="s">
+      <c r="A225" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B225" s="14" t="n">
+      <c r="B225" s="20" t="n">
         <v>7.4</v>
       </c>
       <c r="I225" s="18" t="s">
@@ -8155,10 +8175,10 @@
       <c r="Z225" s="6"/>
     </row>
     <row r="226" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="26" t="s">
+      <c r="A226" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="B226" s="23" t="n">
+      <c r="B226" s="25" t="n">
         <v>0</v>
       </c>
       <c r="I226" s="18" t="s">
@@ -8179,10 +8199,10 @@
       <c r="Z226" s="6"/>
     </row>
     <row r="227" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="26" t="s">
+      <c r="A227" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="B227" s="23" t="n">
+      <c r="B227" s="25" t="n">
         <v>0</v>
       </c>
       <c r="I227" s="18" t="s">

</xml_diff>